<commit_message>
Fixed Label print for according to forwarder.
</commit_message>
<xml_diff>
--- a/public/template/Label-Template.xlsx
+++ b/public/template/Label-Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\mg3h-sp-api\public\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8C3F12-C3E9-405A-B29E-684E7504451B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -18,9 +12,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>AwbNo</t>
   </si>
@@ -38,12 +32,15 @@
   <si>
     <t>BagNo</t>
   </si>
+  <si>
+    <t>Forwarder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,12 +57,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,11 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +149,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,7 +184,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,28 +361,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -388,8 +393,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="54" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="16.149999999999999" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>